<commit_message>
Ricaricamento evidenze per accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#200000SWHCGMXX/COMPUGROUP_MEDICAL_ITALIA_S.R.L/CCBASIC/3.39/report-checklist.xlsx
+++ b/GATEWAY/A1#200000SWHCGMXX/COMPUGROUP_MEDICAL_ITALIA_S.R.L/CCBASIC/3.39/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgm01-my.sharepoint.com/personal/domenico_depinto_cgm_com/Documents/Desktop/validazione/Caricamento SMART/CCBASIC/DA CARICARE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="515" documentId="13_ncr:1_{8E096896-1A5D-440F-9CDB-C984B19F7421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C933C0F3-B963-4226-87CD-0A96C99F594B}"/>
+  <xr:revisionPtr revIDLastSave="524" documentId="13_ncr:1_{8E096896-1A5D-440F-9CDB-C984B19F7421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CFD9D28-8BF1-4CB0-8689-1D7264FD650A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1779,16 +1779,16 @@
     <t>Non è possibile valorizzare il codice in questione con un valore diverso da S quindi l'utente non può mai incorrere in questo errore / scenario</t>
   </si>
   <si>
-    <t>2025-04-29T04:07:05Z</t>
-  </si>
-  <si>
-    <t>70c8f2a5699e9435655c242f94fe0f9d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190203.4.4.9eb93602b302c324f7f812128a82974ebc215f451cdf850428e498734718fded.bc513745d1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Come da email del 13/01/2025 di Segreteria Tecnica FSE - Andrea Di Pietra con oggetto Oggetto: FSE 2.0 - Richiesta di sollecito accreditamento applicativi (cha ha superato il Test 0) , dove si specifica che "il superamento della fase 1 del processo di accreditamento è ritenuto valido se l’applicativo supera almeno il caso di test 1, tra quelli attualmente previsti per il Profilo Sanitario Sintetico sul sito di GitHub Test Case Profilo Sanitario Sintetico."</t>
+  </si>
+  <si>
+    <t>2025-05-13T10:47:40Z</t>
+  </si>
+  <si>
+    <t>ca11b0e6b30257181d5a9a14372fa8c7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190203.4.4.9eb93602b302c324f7f812128a82974ebc215f451cdf850428e498734718fded.1af54dd7cb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2462,6 +2462,27 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2483,27 +2504,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2581,6 +2581,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3953,14 +3957,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:W755"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E155" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C198" sqref="C198"/>
+      <selection pane="bottomRight" activeCell="I168" sqref="I168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4003,12 +4006,12 @@
       <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="48"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="55"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -4029,14 +4032,14 @@
       <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="56" t="s">
+      <c r="B3" s="58"/>
+      <c r="C3" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="55"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -4057,12 +4060,12 @@
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="56" t="s">
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="63" t="s">
         <v>438</v>
       </c>
-      <c r="D4" s="48"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -4084,12 +4087,12 @@
       <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56" t="s">
+      <c r="A5" s="61"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="63" t="s">
         <v>439</v>
       </c>
-      <c r="D5" s="48"/>
+      <c r="D5" s="55"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -4110,8 +4113,8 @@
       <c r="W5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="46"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="10"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -4246,7 +4249,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33">
         <v>4</v>
       </c>
@@ -4283,7 +4286,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35">
         <v>28</v>
       </c>
@@ -4320,7 +4323,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35">
         <v>29</v>
       </c>
@@ -4400,7 +4403,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35">
         <v>31</v>
       </c>
@@ -4437,7 +4440,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35">
         <v>32</v>
       </c>
@@ -4474,7 +4477,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="35">
         <v>33</v>
       </c>
@@ -4511,7 +4514,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="35">
         <v>34</v>
       </c>
@@ -4548,7 +4551,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="35">
         <v>35</v>
       </c>
@@ -4585,7 +4588,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="35">
         <v>36</v>
       </c>
@@ -4622,7 +4625,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="35">
         <v>37</v>
       </c>
@@ -4702,7 +4705,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="35">
         <v>39</v>
       </c>
@@ -4739,7 +4742,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35">
         <v>40</v>
       </c>
@@ -4776,7 +4779,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="35">
         <v>41</v>
       </c>
@@ -4813,7 +4816,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35">
         <v>42</v>
       </c>
@@ -4850,7 +4853,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="35">
         <v>43</v>
       </c>
@@ -4887,7 +4890,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="35">
         <v>44</v>
       </c>
@@ -4926,7 +4929,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="35">
         <v>45</v>
       </c>
@@ -5020,7 +5023,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="35">
         <v>47</v>
       </c>
@@ -5059,7 +5062,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="35">
         <v>48</v>
       </c>
@@ -5098,7 +5101,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="35">
         <v>49</v>
       </c>
@@ -5137,7 +5140,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="35">
         <v>50</v>
       </c>
@@ -5176,7 +5179,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="35">
         <v>51</v>
       </c>
@@ -5215,7 +5218,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="35">
         <v>53</v>
       </c>
@@ -5252,7 +5255,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="35">
         <v>55</v>
       </c>
@@ -5289,7 +5292,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="35">
         <v>56</v>
       </c>
@@ -5326,7 +5329,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="35">
         <v>57</v>
       </c>
@@ -5363,7 +5366,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="35">
         <v>58</v>
       </c>
@@ -5400,7 +5403,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="35">
         <v>59</v>
       </c>
@@ -5437,7 +5440,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="35">
         <v>60</v>
       </c>
@@ -5474,7 +5477,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="35">
         <v>61</v>
       </c>
@@ -5511,7 +5514,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="35">
         <v>62</v>
       </c>
@@ -5548,7 +5551,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="35">
         <v>64</v>
       </c>
@@ -5585,7 +5588,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35">
         <v>66</v>
       </c>
@@ -5622,7 +5625,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="35">
         <v>67</v>
       </c>
@@ -5659,7 +5662,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="35">
         <v>68</v>
       </c>
@@ -5696,7 +5699,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="35">
         <v>69</v>
       </c>
@@ -5733,7 +5736,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="35">
         <v>70</v>
       </c>
@@ -5770,7 +5773,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="35">
         <v>71</v>
       </c>
@@ -5807,7 +5810,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="35">
         <v>72</v>
       </c>
@@ -5844,7 +5847,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="35">
         <v>73</v>
       </c>
@@ -5881,7 +5884,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="35">
         <v>74</v>
       </c>
@@ -5918,7 +5921,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="35">
         <v>76</v>
       </c>
@@ -5955,7 +5958,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="35">
         <v>78</v>
       </c>
@@ -5992,7 +5995,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="35">
         <v>79</v>
       </c>
@@ -6029,7 +6032,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="35">
         <v>80</v>
       </c>
@@ -6066,7 +6069,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="35">
         <v>81</v>
       </c>
@@ -6103,7 +6106,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="35">
         <v>82</v>
       </c>
@@ -6140,7 +6143,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="35">
         <v>83</v>
       </c>
@@ -6177,7 +6180,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="35">
         <v>84</v>
       </c>
@@ -6214,7 +6217,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="35">
         <v>85</v>
       </c>
@@ -6251,7 +6254,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="35">
         <v>86</v>
       </c>
@@ -6288,7 +6291,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="35">
         <v>87</v>
       </c>
@@ -6325,7 +6328,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="35">
         <v>88</v>
       </c>
@@ -6362,7 +6365,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="35">
         <v>89</v>
       </c>
@@ -6399,7 +6402,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="35">
         <v>90</v>
       </c>
@@ -6436,7 +6439,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="35">
         <v>91</v>
       </c>
@@ -6473,7 +6476,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="35">
         <v>92</v>
       </c>
@@ -6510,7 +6513,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="35">
         <v>93</v>
       </c>
@@ -6547,7 +6550,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="35">
         <v>95</v>
       </c>
@@ -6584,7 +6587,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="35">
         <v>97</v>
       </c>
@@ -6621,7 +6624,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="35">
         <v>98</v>
       </c>
@@ -6658,7 +6661,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="35">
         <v>99</v>
       </c>
@@ -6695,7 +6698,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="35">
         <v>100</v>
       </c>
@@ -6732,7 +6735,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="35">
         <v>101</v>
       </c>
@@ -6769,7 +6772,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="35">
         <v>102</v>
       </c>
@@ -6806,7 +6809,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="35">
         <v>103</v>
       </c>
@@ -6843,7 +6846,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="35">
         <v>104</v>
       </c>
@@ -6880,7 +6883,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="35">
         <v>105</v>
       </c>
@@ -6917,7 +6920,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="81" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="35">
         <v>106</v>
       </c>
@@ -6954,7 +6957,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="35">
         <v>108</v>
       </c>
@@ -6991,7 +6994,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="83" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="35">
         <v>110</v>
       </c>
@@ -7028,7 +7031,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="35">
         <v>111</v>
       </c>
@@ -7065,7 +7068,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="35">
         <v>112</v>
       </c>
@@ -7102,7 +7105,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="35">
         <v>113</v>
       </c>
@@ -7139,7 +7142,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="87" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="35">
         <v>114</v>
       </c>
@@ -7176,7 +7179,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="35">
         <v>115</v>
       </c>
@@ -7213,7 +7216,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="35">
         <v>116</v>
       </c>
@@ -7250,7 +7253,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="35">
         <v>117</v>
       </c>
@@ -7287,7 +7290,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="91" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="35">
         <v>118</v>
       </c>
@@ -7324,7 +7327,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="92" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="35">
         <v>119</v>
       </c>
@@ -7361,7 +7364,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="35">
         <v>120</v>
       </c>
@@ -7398,7 +7401,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="94" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="35">
         <v>121</v>
       </c>
@@ -7435,7 +7438,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="35">
         <v>123</v>
       </c>
@@ -7472,7 +7475,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="35">
         <v>125</v>
       </c>
@@ -7509,7 +7512,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="97" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="35">
         <v>126</v>
       </c>
@@ -7546,7 +7549,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="98" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="35">
         <v>127</v>
       </c>
@@ -7583,7 +7586,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="99" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="35">
         <v>128</v>
       </c>
@@ -7620,7 +7623,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="35">
         <v>129</v>
       </c>
@@ -7657,7 +7660,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="101" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="35">
         <v>130</v>
       </c>
@@ -7694,7 +7697,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="35">
         <v>131</v>
       </c>
@@ -7731,7 +7734,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="35">
         <v>132</v>
       </c>
@@ -7768,7 +7771,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="35">
         <v>133</v>
       </c>
@@ -7805,7 +7808,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="105" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="35">
         <v>134</v>
       </c>
@@ -7842,7 +7845,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="106" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="35">
         <v>135</v>
       </c>
@@ -7879,7 +7882,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="35">
         <v>136</v>
       </c>
@@ -7916,7 +7919,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="108" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="35">
         <v>137</v>
       </c>
@@ -7953,7 +7956,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="35">
         <v>138</v>
       </c>
@@ -7990,7 +7993,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="35">
         <v>139</v>
       </c>
@@ -8027,7 +8030,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="111" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="35">
         <v>140</v>
       </c>
@@ -8064,7 +8067,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="112" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="35">
         <v>141</v>
       </c>
@@ -8101,7 +8104,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="113" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="35">
         <v>142</v>
       </c>
@@ -8138,7 +8141,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="114" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="35">
         <v>143</v>
       </c>
@@ -8175,7 +8178,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="115" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="35">
         <v>144</v>
       </c>
@@ -8212,7 +8215,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="116" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="35">
         <v>145</v>
       </c>
@@ -8249,7 +8252,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="117" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="35">
         <v>146</v>
       </c>
@@ -8286,7 +8289,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="118" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="35">
         <v>152</v>
       </c>
@@ -8323,7 +8326,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="119" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="35">
         <v>154</v>
       </c>
@@ -8360,7 +8363,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="120" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="35">
         <v>155</v>
       </c>
@@ -8397,7 +8400,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="121" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="35">
         <v>156</v>
       </c>
@@ -8434,7 +8437,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="122" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="35">
         <v>158</v>
       </c>
@@ -8471,7 +8474,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="35">
         <v>159</v>
       </c>
@@ -8508,7 +8511,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="35">
         <v>160</v>
       </c>
@@ -8545,7 +8548,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="35">
         <v>161</v>
       </c>
@@ -8582,7 +8585,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="126" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="35">
         <v>162</v>
       </c>
@@ -8619,7 +8622,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="127" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="35">
         <v>163</v>
       </c>
@@ -8656,7 +8659,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="35">
         <v>164</v>
       </c>
@@ -8693,7 +8696,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="129" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="35">
         <v>165</v>
       </c>
@@ -8730,7 +8733,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="130" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="35">
         <v>166</v>
       </c>
@@ -8767,7 +8770,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="131" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="35">
         <v>167</v>
       </c>
@@ -8804,7 +8807,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="132" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="35">
         <v>168</v>
       </c>
@@ -8841,7 +8844,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="133" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="35">
         <v>169</v>
       </c>
@@ -8947,7 +8950,7 @@
       <c r="K135" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="L135" s="57" t="s">
+      <c r="L135" s="45" t="s">
         <v>445</v>
       </c>
       <c r="M135" s="38"/>
@@ -8990,7 +8993,7 @@
       <c r="K136" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="L136" s="57" t="s">
+      <c r="L136" s="45" t="s">
         <v>446</v>
       </c>
       <c r="M136" s="38"/>
@@ -9033,7 +9036,7 @@
       <c r="K137" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="L137" s="57" t="s">
+      <c r="L137" s="45" t="s">
         <v>447</v>
       </c>
       <c r="M137" s="38"/>
@@ -9076,7 +9079,7 @@
       <c r="K138" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="L138" s="57" t="s">
+      <c r="L138" s="45" t="s">
         <v>448</v>
       </c>
       <c r="M138" s="38"/>
@@ -9119,7 +9122,7 @@
       <c r="K139" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="L139" s="57" t="s">
+      <c r="L139" s="45" t="s">
         <v>449</v>
       </c>
       <c r="M139" s="38"/>
@@ -9162,7 +9165,7 @@
       <c r="K140" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="L140" s="57" t="s">
+      <c r="L140" s="45" t="s">
         <v>450</v>
       </c>
       <c r="M140" s="38"/>
@@ -9205,7 +9208,7 @@
       <c r="K141" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="L141" s="57" t="s">
+      <c r="L141" s="45" t="s">
         <v>451</v>
       </c>
       <c r="M141" s="38"/>
@@ -9248,7 +9251,7 @@
       <c r="K142" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="L142" s="57" t="s">
+      <c r="L142" s="45" t="s">
         <v>452</v>
       </c>
       <c r="M142" s="38"/>
@@ -9291,7 +9294,7 @@
       <c r="K143" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="L143" s="57" t="s">
+      <c r="L143" s="45" t="s">
         <v>453</v>
       </c>
       <c r="M143" s="38"/>
@@ -9334,7 +9337,7 @@
       <c r="K144" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="L144" s="57" t="s">
+      <c r="L144" s="45" t="s">
         <v>454</v>
       </c>
       <c r="M144" s="38"/>
@@ -9377,7 +9380,7 @@
       <c r="K145" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="L145" s="57" t="s">
+      <c r="L145" s="45" t="s">
         <v>455</v>
       </c>
       <c r="M145" s="38"/>
@@ -9420,7 +9423,7 @@
       <c r="K146" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="L146" s="57" t="s">
+      <c r="L146" s="45" t="s">
         <v>456</v>
       </c>
       <c r="M146" s="38"/>
@@ -9463,7 +9466,7 @@
       <c r="K147" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="L147" s="57" t="s">
+      <c r="L147" s="45" t="s">
         <v>457</v>
       </c>
       <c r="M147" s="38"/>
@@ -9506,7 +9509,7 @@
       <c r="K148" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="L148" s="57" t="s">
+      <c r="L148" s="45" t="s">
         <v>458</v>
       </c>
       <c r="M148" s="38"/>
@@ -9523,7 +9526,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="149" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="35">
         <v>191</v>
       </c>
@@ -9560,7 +9563,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="150" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="35">
         <v>376</v>
       </c>
@@ -9597,7 +9600,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="151" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="35">
         <v>417</v>
       </c>
@@ -9634,7 +9637,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="152" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="35">
         <v>418</v>
       </c>
@@ -9671,7 +9674,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="153" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="35">
         <v>419</v>
       </c>
@@ -9708,7 +9711,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="154" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="35">
         <v>423</v>
       </c>
@@ -9745,7 +9748,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="155" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="35">
         <v>424</v>
       </c>
@@ -9782,7 +9785,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="156" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="35">
         <v>425</v>
       </c>
@@ -9819,7 +9822,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="157" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="35">
         <v>432</v>
       </c>
@@ -9856,7 +9859,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="158" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="35">
         <v>433</v>
       </c>
@@ -9893,7 +9896,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="159" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="35">
         <v>434</v>
       </c>
@@ -9930,7 +9933,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="160" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="35">
         <v>435</v>
       </c>
@@ -9967,7 +9970,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="161" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="35">
         <v>437</v>
       </c>
@@ -10004,7 +10007,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="162" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="35">
         <v>438</v>
       </c>
@@ -10041,7 +10044,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="163" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="35">
         <v>440</v>
       </c>
@@ -10078,7 +10081,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="164" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="35">
         <v>441</v>
       </c>
@@ -10115,7 +10118,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="165" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="35">
         <v>442</v>
       </c>
@@ -10152,7 +10155,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="166" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="35">
         <v>443</v>
       </c>
@@ -10205,34 +10208,34 @@
       <c r="E167" s="43" t="s">
         <v>247</v>
       </c>
-      <c r="F167" s="58">
-        <v>45776</v>
-      </c>
-      <c r="G167" s="59" t="s">
-        <v>459</v>
-      </c>
-      <c r="H167" s="59" t="s">
+      <c r="F167" s="46">
+        <v>45790</v>
+      </c>
+      <c r="G167" s="47" t="s">
         <v>460</v>
       </c>
-      <c r="I167" s="59" t="s">
+      <c r="H167" s="47" t="s">
         <v>461</v>
       </c>
-      <c r="J167" s="60" t="s">
+      <c r="I167" s="47" t="s">
+        <v>462</v>
+      </c>
+      <c r="J167" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="K167" s="60"/>
-      <c r="L167" s="60"/>
-      <c r="M167" s="60"/>
-      <c r="N167" s="60"/>
-      <c r="O167" s="60"/>
-      <c r="P167" s="60"/>
-      <c r="Q167" s="60"/>
-      <c r="R167" s="60"/>
-      <c r="S167" s="60"/>
-      <c r="T167" s="60"/>
-      <c r="U167" s="61"/>
-      <c r="V167" s="62"/>
-      <c r="W167" s="63" t="s">
+      <c r="K167" s="48"/>
+      <c r="L167" s="48"/>
+      <c r="M167" s="48"/>
+      <c r="N167" s="48"/>
+      <c r="O167" s="48"/>
+      <c r="P167" s="48"/>
+      <c r="Q167" s="48"/>
+      <c r="R167" s="48"/>
+      <c r="S167" s="48"/>
+      <c r="T167" s="48"/>
+      <c r="U167" s="49"/>
+      <c r="V167" s="50"/>
+      <c r="W167" s="51" t="s">
         <v>36</v>
       </c>
     </row>
@@ -10263,7 +10266,7 @@
         <v>243</v>
       </c>
       <c r="L168" s="38" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="M168" s="38"/>
       <c r="N168" s="38"/>
@@ -10279,7 +10282,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="169" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="35">
         <v>448</v>
       </c>
@@ -10316,7 +10319,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="170" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="35">
         <v>449</v>
       </c>
@@ -10353,7 +10356,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="171" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="35">
         <v>450</v>
       </c>
@@ -10390,7 +10393,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="172" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="35">
         <v>451</v>
       </c>
@@ -10427,7 +10430,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="173" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="35">
         <v>452</v>
       </c>
@@ -10464,7 +10467,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="174" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="35">
         <v>454</v>
       </c>
@@ -10501,7 +10504,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="175" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="35">
         <v>455</v>
       </c>
@@ -10538,7 +10541,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="176" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="35">
         <v>456</v>
       </c>
@@ -10575,7 +10578,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="177" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="35">
         <v>457</v>
       </c>
@@ -10612,7 +10615,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="178" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="35">
         <v>458</v>
       </c>
@@ -10649,7 +10652,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="179" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="35">
         <v>459</v>
       </c>
@@ -10686,7 +10689,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="35">
         <v>460</v>
       </c>
@@ -10723,7 +10726,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="181" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="35">
         <v>461</v>
       </c>
@@ -10760,7 +10763,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="182" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="35">
         <v>462</v>
       </c>
@@ -10797,7 +10800,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="183" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="35">
         <v>463</v>
       </c>
@@ -10834,7 +10837,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="184" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="35">
         <v>464</v>
       </c>
@@ -10871,7 +10874,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="35">
         <v>465</v>
       </c>
@@ -10908,7 +10911,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="186" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="35">
         <v>466</v>
       </c>
@@ -10945,7 +10948,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="35">
         <v>467</v>
       </c>
@@ -10982,7 +10985,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="188" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="35">
         <v>468</v>
       </c>
@@ -11046,7 +11049,7 @@
         <v>243</v>
       </c>
       <c r="L189" s="38" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="M189" s="35"/>
       <c r="N189" s="35"/>
@@ -11062,7 +11065,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="190" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="35">
         <v>470</v>
       </c>
@@ -11099,7 +11102,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="191" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="35">
         <v>471</v>
       </c>
@@ -11136,7 +11139,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="192" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="35">
         <v>472</v>
       </c>
@@ -15250,13 +15253,7 @@
     <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A9:W192" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="PSS"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A9:W192" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>

</xml_diff>